<commit_message>
updated tests + sorting now matches amibroker for portfolio
</commit_message>
<xml_diff>
--- a/Tests/baseline_short_sma_5_25_JPM.xlsx
+++ b/Tests/baseline_short_sma_5_25_JPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Windows\Documents\bt_plat\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9A231-E4F2-4580-BAE7-B7F96CCF73E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643EEF6A-1188-46B9-85BB-4DF89C555DC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15667,8 +15667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC41757A-AC97-41E0-ADEC-9FB26D7A223F}">
   <dimension ref="A1:P287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17785,7 +17785,7 @@
         <v>8.83</v>
       </c>
       <c r="G53" s="2">
-        <v>0.1037</v>
+        <v>0.1038</v>
       </c>
       <c r="H53">
         <v>-102.09</v>
@@ -19865,13 +19865,13 @@
         <v>8.25</v>
       </c>
       <c r="G105" s="2">
-        <v>3.1300000000000001E-2</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="H105">
         <v>-30.25</v>
       </c>
       <c r="I105" s="2">
-        <v>-3.1300000000000001E-2</v>
+        <v>-3.1199999999999999E-2</v>
       </c>
       <c r="J105">
         <v>121</v>

</xml_diff>